<commit_message>
Add new param to exel and test new excel format
</commit_message>
<xml_diff>
--- a/public/xls/Admin/Admin User/Mockup(Admin User).xlsx
+++ b/public/xls/Admin/Admin User/Mockup(Admin User).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="555" windowWidth="20775" windowHeight="9660"/>
+    <workbookView xWindow="270" yWindow="555" windowWidth="20775" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Exam grades" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -171,12 +171,6 @@
     <t>Кушнір Андрій Олегович</t>
   </si>
   <si>
-    <t>TestListID</t>
-  </si>
-  <si>
-    <t>DisciplineID</t>
-  </si>
-  <si>
     <t>DisciplineVariantID</t>
   </si>
   <si>
@@ -189,12 +183,6 @@
     <t>NameModule</t>
   </si>
   <si>
-    <t>12010000171334</t>
-  </si>
-  <si>
-    <t>1794</t>
-  </si>
-  <si>
     <t>12010000137215</t>
   </si>
   <si>
@@ -217,6 +205,36 @@
   </si>
   <si>
     <t>module_num</t>
+  </si>
+  <si>
+    <t>EduYear</t>
+  </si>
+  <si>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>DepartmentId</t>
+  </si>
+  <si>
+    <t>SpecialityId</t>
+  </si>
+  <si>
+    <t>ModuleNum</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -250,9 +268,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -559,7 +578,7 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -567,16 +586,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -590,7 +609,7 @@
         <v>12345</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -632,7 +651,7 @@
         <v>12348</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -674,7 +693,7 @@
         <v>12351</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -702,7 +721,7 @@
         <v>12353</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,7 +749,7 @@
         <v>12355</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -758,7 +777,7 @@
         <v>12357</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -786,7 +805,7 @@
         <v>12359</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1224,9 +1243,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1238,44 +1259,62 @@
     <col min="6" max="6" width="57.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s">
+      <c r="I2" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upd prefer data to create documents and Statistics
</commit_message>
<xml_diff>
--- a/public/xls/Admin/Admin User/Mockup(Admin User).xlsx
+++ b/public/xls/Admin/Admin User/Mockup(Admin User).xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schekanov\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7260"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Table decode" sheetId="2" r:id="rId2"/>
     <sheet name="Table Info" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1089,8 +1094,8 @@
   </sheetPr>
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2499,7 +2504,7 @@
   <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>